<commit_message>
FeatureRM #382 (amp_squid): Add debug variant tests (*.json) and create 2 test name in order to:   . loop on all debug variant tests   . loop on all functionnal variant tests.
</commit_message>
<xml_diff>
--- a/simu/conf/fpasim/amp_squid/amp_squid_top_test_list.xlsx
+++ b/simu/conf/fpasim/amp_squid/amp_squid_top_test_list.xlsx
@@ -31,6 +31,9 @@
       <style:table-column-properties fo:break-before="auto" style:column-width="6.371cm"/>
     </style:style>
     <style:style style:name="co4" style:family="table-column">
+      <style:table-column-properties fo:break-before="auto" style:column-width="8.523cm"/>
+    </style:style>
+    <style:style style:name="co5" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="2.258cm"/>
     </style:style>
     <style:style style:name="ro1" style:family="table-row">
@@ -45,8 +48,9 @@
     <style:style style:name="ta1" style:family="table" style:master-page-name="Default">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
     </style:style>
-    <style:style style:name="ce1" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="#00a933"/>
+    <style:style style:name="ce5" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:background-color="#00a933" style:text-align-source="fix" style:repeat-content="false" style:vertical-align="middle"/>
+      <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
     </style:style>
     <style:style style:name="ce2" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" style:vertical-align="middle"/>
@@ -69,34 +73,54 @@
     <style:style style:name="ce11" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:background-color="#808080" style:vertical-align="top"/>
     </style:style>
+    <style:style style:name="ce15" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" style:vertical-align="middle"/>
+      <style:paragraph-properties fo:text-align="center"/>
+    </style:style>
+    <style:style style:name="ce16" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:wrap-option="wrap"/>
+    </style:style>
     <style:style style:name="T1" style:family="text">
       <style:text-properties style:font-name="Liberation Sans" fo:font-size="10pt" fo:font-weight="normal" style:text-underline-style="none" style:text-underline-color="font-color" style:text-line-through-type="none" fo:font-style="normal" style:text-outline="false" fo:text-shadow="none" style:text-line-through-mode="continuous" fo:language="fr" fo:country="FR" style:language-asian="zh" style:country-asian="CN" style:language-complex="hi" style:country-complex="IN" style:font-name-asian="Microsoft YaHei" style:font-name-complex="Arial" style:font-size-asian="10pt" style:font-size-complex="10pt" style:font-weight-asian="normal" style:font-weight-complex="normal" style:font-style-asian="normal" style:font-style-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
+    </style:style>
+    <style:style style:name="T2" style:family="text">
+      <style:text-properties fo:color="#c9211e"/>
+    </style:style>
+    <style:style style:name="T3" style:family="text">
+      <style:text-properties fo:color="#000000"/>
+    </style:style>
+    <style:style style:name="T4" style:family="text">
+      <style:text-properties fo:color="#ff0000"/>
     </style:style>
   </office:automatic-styles>
   <office:body>
     <office:spreadsheet>
       <table:table table:name="Feuille1" table:style-name="ta1">
         <table:table-column table:style-name="co1" table:default-cell-style-name="ce2"/>
-        <table:table-column table:style-name="co2" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co2" table:default-cell-style-name="ce3"/>
         <table:table-column table:style-name="co3" table:default-cell-style-name="ce4"/>
-        <table:table-column table:style-name="co4" table:number-columns-repeated="1021" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co4" table:default-cell-style-name="ce16"/>
+        <table:table-column table:style-name="co5" table:number-columns-repeated="1020" table:default-cell-style-name="Default"/>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>test_name</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>parameters summary</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
+            <text:p>reading speed</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>comment</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
+          <table:table-cell table:number-columns-repeated="1020"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>tb_amp_squid_top_test_variant_func00.json</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>« fpasim »:1,</text:p>
             <text:p>
               <text:span text:style-name="T1">"nb_sample_by_pixel": 40,</text:span>
@@ -134,13 +158,16 @@
             <text:p>Continuous ram1 check</text:p>
             <text:p/>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+            <text:p>Nominal case</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>tb_amp_squid_top_test_variant_func01.json</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>« fpasim »:1,</text:p>
             <text:p>
               <text:span text:style-name="T1">"nb_sample_by_pixel": 40,</text:span>
@@ -178,13 +205,16 @@
             <text:p>Continuous ram1 check</text:p>
             <text:p/>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+            <text:p>Low limit case</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>tb_amp_squid_top_test_variant_func02.json</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>« fpasim »:1,</text:p>
             <text:p>
               <text:span text:style-name="T1">"nb_sample_by_pixel": 40,</text:span>
@@ -222,7 +252,10 @@
             <text:p>Continuous ram1 check</text:p>
             <text:p/>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+            <text:p>High limite case</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell table:style-name="ce7"/>
@@ -234,8 +267,8 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>tb_amp_squid_top_test_variant_debug00.json</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
-            <text:p>« fpasim »:1,</text:p>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>« fpasim »:0,</text:p>
             <text:p>
               <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
             </text:p>
@@ -272,22 +305,506 @@
             <text:p>Continuous ram1 check</text:p>
             <text:p/>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1" table:number-rows-repeated="7">
-          <table:table-cell table:number-columns-repeated="1024"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1" table:number-rows-repeated="2">
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+            <text:p>Short simulation</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tb_amp_squid_top_test_variant_debug01.json</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>« fpasim »:0,</text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pixel_by_frame": 2,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_frame_by_pulse": 3,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pulse": 2,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ « mode »:0,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ «min_value »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ « max_value »:10,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « mode »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « min_value »:10,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « max_value »:20</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Continuous data valid</text:p>
+            <text:p>
+              <text:span text:style-name="T4">Sporadic ram1 check</text:span>
+            </text:p>
+            <text:p/>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+            <text:p>Sporadic Writting RAM</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tb_amp_squid_top_test_variant_debug02.json</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T2">« fpasim »:0,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pixel_by_frame": 34,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_frame_by_pulse": 2048,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pulse": 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ « mode »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ «min_value »:-8192,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ « max_value »:8191,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « mode »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « min_value »:-131072,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « max_value »:131071</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Continuous data valid</text:p>
+            <text:p>Continuous ram1 check</text:p>
+            <text:p/>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="8">
+            <text:p>fpasim variation</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tb_amp_squid_top_test_variant_debug03.json</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T2">« fpasim »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pixel_by_frame": 34,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_frame_by_pulse": 2048,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pulse": 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ « mode »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ «min_value »:-8192,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ « max_value »:8191,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « mode »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « min_value »:-131072,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « max_value »:131071</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Continuous data valid</text:p>
+            <text:p>Continuous ram1 check</text:p>
+            <text:p/>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tb_amp_squid_top_test_variant_debug04.json</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T2">« fpasim »:2,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pixel_by_frame": 34,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_frame_by_pulse": 2048,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pulse": 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ « mode »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ «min_value »:-8192,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ « max_value »:8191,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « mode »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « min_value »:-131072,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « max_value »:131071</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Continuous data valid</text:p>
+            <text:p>Continuous ram1 check</text:p>
+            <text:p/>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tb_amp_squid_top_test_variant_debug05.json</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T2">« fpasim »:3,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pixel_by_frame": 34,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_frame_by_pulse": 2048,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pulse": 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ « mode »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ «min_value »:-8192,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ « max_value »:8191,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « mode »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « min_value »:-131072,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « max_value »:131071</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Continuous data valid</text:p>
+            <text:p>Continuous ram1 check</text:p>
+            <text:p/>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tb_amp_squid_top_test_variant_debug06.json</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T2">« fpasim »:4,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pixel_by_frame": 34,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_frame_by_pulse": 2048,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pulse": 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ « mode »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ «min_value »:-8192,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ « max_value »:8191,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « mode »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « min_value »:-131072,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « max_value »:131071</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Continuous data valid</text:p>
+            <text:p>Continuous ram1 check</text:p>
+            <text:p/>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tb_amp_squid_top_test_variant_debug07.json</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T2">« fpasim »:5,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pixel_by_frame": 34,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_frame_by_pulse": 2048,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pulse": 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ « mode »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ «min_value »:-8192,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ « max_value »:8191,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « mode »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « min_value »:-131072,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « max_value »:131071</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Continuous data valid</text:p>
+            <text:p>Continuous ram1 check</text:p>
+            <text:p/>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tb_amp_squid_top_test_variant_debug08.json</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T2">« fpasim »:6,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pixel_by_frame": 34,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_frame_by_pulse": 2048,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pulse": 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ « mode »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ «min_value »:-8192,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ « max_value »:8191,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « mode »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « min_value »:-131072,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « max_value »:131071</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Continuous data valid</text:p>
+            <text:p>Continuous ram1 check</text:p>
+            <text:p/>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tb_amp_squid_top_test_variant_debug09.json</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T2">« fpasim »:7,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pixel_by_frame": 34,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_frame_by_pulse": 2048,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pulse": 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ « mode »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ «min_value »:-8192,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ « max_value »:8191,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « mode »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « min_value »:-131072,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « max_value »:131071</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Continuous data valid</text:p>
+            <text:p>Continuous ram1 check</text:p>
+            <text:p/>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tb_amp_squid_top_test_variant_debug10.json</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T3">« fpasim »:0,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_sample_by_pixel": 8,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pixel_by_frame": 34,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_frame_by_pulse": 2048,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"nb_pulse": 1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ « mode »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ «min_value »:-8192,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">"amp_squid_offset_correction"/ « max_value »:8191,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « mode »:1,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « min_value »:-131072,</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">« pixel_result »/ « max_value »:131071</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T4">sporadic data valid</text:span>
+            </text:p>
+            <text:p>Continuous ram1 check</text:p>
+            <text:p/>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+            <text:p>Data input stream test (non nominal case)</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:style-name="Default" table:number-columns-repeated="4"/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
           <table:table-cell table:style-name="Default"/>
           <table:table-cell/>
           <table:table-cell table:style-name="Default"/>
-          <table:table-cell table:number-columns-repeated="1021"/>
+          <table:table-cell table:number-columns-repeated="1020"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="1024"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="1024"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="Default"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="Default"/>
+          <table:table-cell table:number-columns-repeated="1020"/>
         </table:table-row>
       </table:table>
       <table:named-expressions/>
@@ -299,11 +816,11 @@
 <file path=meta.xml><?xml version="1.0" encoding="utf-8"?>
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" office:version="1.3">
   <office:meta>
-    <dc:date>2023-05-30T13:57:12.740000000</dc:date>
-    <meta:editing-duration>PT1H43M11S</meta:editing-duration>
-    <meta:editing-cycles>11</meta:editing-cycles>
+    <dc:date>2023-06-02T09:00:26.960000000</dc:date>
+    <meta:editing-duration>PT3H7M19S</meta:editing-duration>
+    <meta:editing-cycles>15</meta:editing-cycles>
     <meta:generator>LibreOffice/7.2.4.1$Windows_X86_64 LibreOffice_project/27d75539669ac387bb498e35313b970b7fe9c4f9</meta:generator>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="15" meta:object-count="0"/>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="53" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -314,15 +831,15 @@
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">24533</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">18822</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">33057</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">62778</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Feuille1">
-              <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">1</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">5</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">6</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -331,7 +848,7 @@
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
-              <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">3</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
               <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -375,6 +892,15 @@
       <config:config-item config:name="EmbedFonts" config:type="boolean">false</config:config-item>
       <config:config-item config:name="EmbedLatinScriptFonts" config:type="boolean">true</config:config-item>
       <config:config-item config:name="EmbedOnlyUsedFonts" config:type="boolean">false</config:config-item>
+      <config:config-item-map-indexed config:name="ForbiddenCharacters">
+        <config:config-item-map-entry>
+          <config:config-item config:name="Language" config:type="string">fr</config:config-item>
+          <config:config-item config:name="Country" config:type="string">FR</config:config-item>
+          <config:config-item config:name="Variant" config:type="string"/>
+          <config:config-item config:name="BeginLine" config:type="string"/>
+          <config:config-item config:name="EndLine" config:type="string"/>
+        </config:config-item-map-entry>
+      </config:config-item-map-indexed>
       <config:config-item config:name="GridColor" config:type="int">12632256</config:config-item>
       <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
       <config:config-item config:name="HasSheetTabs" config:type="boolean">true</config:config-item>
@@ -543,9 +1069,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2023-05-30">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2023-06-02">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="13:52:49.432000000">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="07:34:12.452000000">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>

<commit_message>
amp, ci: rename *_debug10.json into *_debug03.json.
</commit_message>
<xml_diff>
--- a/simu/conf/fpasim/amp_squid/amp_squid_top_test_list.xlsx
+++ b/simu/conf/fpasim/amp_squid/amp_squid_top_test_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fpasim-fw-hardware\simu\conf\fpasim\amp_squid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7257644C-7585-4D2A-B8B3-FCFB57709B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3E5B01-FFC4-42C9-9F57-B31A52584677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,9 +62,6 @@
     <t>tb_amp_squid_top_test_variant_debug02.json</t>
   </si>
   <si>
-    <t>tb_amp_squid_top_test_variant_debug10.json</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Continuous data valid
 </t>
@@ -410,6 +407,9 @@
 « pixel_result »/ « min_value »:-131072,
 « pixel_result »/ « max_value »:131071</t>
     </r>
+  </si>
+  <si>
+    <t>tb_amp_squid_top_test_variant_debug03.json</t>
   </si>
 </sst>
 </file>
@@ -787,7 +787,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,13 +817,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="225" x14ac:dyDescent="0.25">
@@ -831,13 +831,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="225" x14ac:dyDescent="0.25">
@@ -845,13 +845,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -865,13 +865,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="225" x14ac:dyDescent="0.25">
@@ -879,13 +879,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="225" x14ac:dyDescent="0.25">
@@ -893,33 +893,33 @@
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="225" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ci,amp: add the tb_amp_squid_top_test_variant_debug04.json test: disable the adc input and increment the second input in order to output the memory content.
</commit_message>
<xml_diff>
--- a/simu/conf/fpasim/amp_squid/amp_squid_top_test_list.xlsx
+++ b/simu/conf/fpasim/amp_squid/amp_squid_top_test_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fpasim-fw-hardware\simu\conf\fpasim\amp_squid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3E5B01-FFC4-42C9-9F57-B31A52584677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7307859-6562-4D5F-83B5-F65CD787A49B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5880" yWindow="2055" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>test_name</t>
   </si>
@@ -410,6 +410,71 @@
   </si>
   <si>
     <t>tb_amp_squid_top_test_variant_debug03.json</t>
+  </si>
+  <si>
+    <t>tb_amp_squid_top_test_variant_debug04.json</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"nb_sample_by_pixel": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,
+"nb_pixel_by_frame": 1,
+"nb_frame_by_pulse": 2048,
+"nb_pulse": 8,
+"amp_squid_offset_correction"/ « mode »:0,
+"amp_squid_offset_correction"/ «min_value »:0,
+"amp_squid_offset_correction"/ « max_value »:0,
+« pixel_result »/ « mode »:0,
+« pixel_result »/ « min_value »:0,
+« pixel_result »/ « max_value »:131071</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Liberation Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Continuous data valid
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Continuous ram1 check
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Auto-check
+disable adc data (=0) to read the memory content
+1 pixel by frame</t>
   </si>
 </sst>
 </file>
@@ -786,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,6 +981,20 @@
         <v>20</v>
       </c>
     </row>
+    <row r="10" spans="1:4" ht="225" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="13" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="10" t="s">

</xml_diff>

<commit_message>
ci, amp: minor update
</commit_message>
<xml_diff>
--- a/simu/conf/fpasim/amp_squid/amp_squid_top_test_list.xlsx
+++ b/simu/conf/fpasim/amp_squid/amp_squid_top_test_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fpasim-fw-hardware\simu\conf\fpasim\amp_squid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7307859-6562-4D5F-83B5-F65CD787A49B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED43A623-7191-4C51-B569-172C55F526F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="2055" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -473,7 +473,7 @@
   </si>
   <si>
     <t>Auto-check
-disable adc data (=0) to read the memory content
+disable adc data (=0) =&gt; output the memory content (non nominal case)
 1 pixel by frame</t>
   </si>
 </sst>

</xml_diff>